<commit_message>
UC, add data of minimum duration time
</commit_message>
<xml_diff>
--- a/ams/cases/ieee14/ieee14_uc.xlsx
+++ b/ams/cases/ieee14/ieee14_uc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10514"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\jwang\work\ams\ams\cases\ieee14\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinningwang/Documents/work/ams/ams/cases/ieee14/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E24AEB99-0FE6-43E2-83C2-DB4FF9D58A3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B515F621-CDB8-C743-BDAD-20E2A6D3B033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2160" yWindow="2550" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="1540" windowWidth="34560" windowHeight="19000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="12" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1044" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1048" uniqueCount="270">
   <si>
     <t>uid</t>
   </si>
@@ -798,35 +798,35 @@
   </si>
   <si>
     <t>for UC, ED</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>1, 1</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>1, 1</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>1.005, 1.005</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>1.01, 1.01</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>1.015, 1.015</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>1.02, 1.02</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>1.025, 1.025</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>SLOT1</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>SLOT2</t>
@@ -842,31 +842,44 @@
   </si>
   <si>
     <t>SLOT6</t>
+  </si>
+  <si>
+    <t>td1</t>
+  </si>
+  <si>
+    <t>td2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -874,33 +887,33 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -967,30 +980,39 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1336,9 +1358,9 @@
       <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1356,7 +1378,7 @@
       </c>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>0</v>
       </c>
@@ -1373,7 +1395,7 @@
       <c r="F2" s="5"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1386,9 +1408,9 @@
       <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1402,7 +1424,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1416,7 +1438,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1431,7 +1453,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
@@ -1445,9 +1467,9 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1458,7 +1480,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1469,7 +1491,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1480,7 +1502,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -1491,7 +1513,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -1502,7 +1524,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -1513,7 +1535,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -1525,7 +1547,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1535,12 +1557,12 @@
   <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1584,7 +1606,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1628,7 +1650,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1672,7 +1694,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -1716,7 +1738,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -1760,7 +1782,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -1804,7 +1826,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -1848,7 +1870,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -1892,7 +1914,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>44</v>
       </c>
@@ -1936,7 +1958,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -1980,7 +2002,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>52</v>
       </c>
@@ -2024,7 +2046,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>56</v>
       </c>
@@ -2068,7 +2090,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>60</v>
       </c>
@@ -2112,7 +2134,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>64</v>
       </c>
@@ -2156,7 +2178,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>68</v>
       </c>
@@ -2201,7 +2223,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <ignoredErrors>
@@ -2212,18 +2234,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:T5"/>
+  <dimension ref="A1:V5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+      <selection activeCell="W23" sqref="W23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="20" max="20" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2284,8 +2306,14 @@
       <c r="T1" s="7" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U1" s="13" t="s">
+        <v>268</v>
+      </c>
+      <c r="V1" s="13" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -2343,8 +2371,14 @@
       <c r="T2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U2" s="1">
+        <v>30</v>
+      </c>
+      <c r="V2" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -2402,8 +2436,14 @@
       <c r="T3" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U3" s="1">
+        <v>45</v>
+      </c>
+      <c r="V3" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -2461,8 +2501,14 @@
       <c r="T4" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U4" s="1">
+        <v>40</v>
+      </c>
+      <c r="V4" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -2520,9 +2566,15 @@
       <c r="T5" s="1">
         <v>1</v>
       </c>
+      <c r="U5" s="1">
+        <v>35</v>
+      </c>
+      <c r="V5" s="1">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="A1:S5" numberStoredAsText="1"/>
@@ -2532,18 +2584,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:U2"/>
+  <dimension ref="A1:W2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="21" max="21" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2607,8 +2659,14 @@
       <c r="U1" s="7" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="V1" s="11" t="s">
+        <v>268</v>
+      </c>
+      <c r="W1" s="11" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -2669,9 +2727,15 @@
       <c r="U2" s="8">
         <v>1</v>
       </c>
+      <c r="V2" s="12">
+        <v>50</v>
+      </c>
+      <c r="W2" s="12">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="A1:T2" numberStoredAsText="1"/>
@@ -2685,9 +2749,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2722,7 +2786,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -2757,7 +2821,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -2792,7 +2856,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -2827,7 +2891,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -2862,7 +2926,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -2897,7 +2961,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -2932,7 +2996,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -2967,7 +3031,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>44</v>
       </c>
@@ -3002,7 +3066,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -3037,7 +3101,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>52</v>
       </c>
@@ -3072,7 +3136,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>56</v>
       </c>
@@ -3108,7 +3172,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="A1:K12" numberStoredAsText="1"/>
@@ -3124,9 +3188,9 @@
       <selection activeCell="W12" sqref="W12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3203,7 +3267,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -3271,7 +3335,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -3339,7 +3403,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -3407,7 +3471,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -3475,7 +3539,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -3543,7 +3607,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -3611,7 +3675,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -3679,7 +3743,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>44</v>
       </c>
@@ -3747,7 +3811,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -3815,7 +3879,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>52</v>
       </c>
@@ -3883,7 +3947,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>56</v>
       </c>
@@ -3951,7 +4015,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>60</v>
       </c>
@@ -4019,7 +4083,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>64</v>
       </c>
@@ -4087,7 +4151,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>68</v>
       </c>
@@ -4155,7 +4219,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>72</v>
       </c>
@@ -4223,7 +4287,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>209</v>
       </c>
@@ -4291,7 +4355,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>213</v>
       </c>
@@ -4359,7 +4423,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>217</v>
       </c>
@@ -4427,7 +4491,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>220</v>
       </c>
@@ -4495,7 +4559,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>223</v>
       </c>
@@ -4564,7 +4628,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="A1:X21" numberStoredAsText="1"/>
@@ -4578,9 +4642,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4612,7 +4676,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -4644,7 +4708,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -4677,7 +4741,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="A1:J3" numberStoredAsText="1"/>
@@ -4693,9 +4757,9 @@
       <selection activeCell="D3" sqref="A1:D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4709,7 +4773,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -4723,7 +4787,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -4738,7 +4802,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="A1:D3" numberStoredAsText="1"/>
@@ -4754,9 +4818,9 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4785,7 +4849,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -4814,7 +4878,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -4843,7 +4907,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -4872,7 +4936,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -4901,7 +4965,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -4931,7 +4995,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="A1:D1 G1:I1 A6:D6 A2:D2 G2:I2 A3:D3 G3:I3 A4:D4 G4:I4 A5:D5 G5:I5 G6:I6" numberStoredAsText="1"/>

</xml_diff>

<commit_message>
Add timeslot model for UC and ED
</commit_message>
<xml_diff>
--- a/ams/cases/ieee14/ieee14_uc.xlsx
+++ b/ams/cases/ieee14/ieee14_uc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinningwang/Documents/work/ams/ams/cases/ieee14/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B515F621-CDB8-C743-BDAD-20E2A6D3B033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60FD8622-7260-EE4F-A149-1E2B3811DC88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1540" windowWidth="34560" windowHeight="19000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-36480" yWindow="1540" windowWidth="34560" windowHeight="19000" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="12" r:id="rId1"/>
@@ -23,14 +23,15 @@
     <sheet name="Area" sheetId="7" r:id="rId8"/>
     <sheet name="GCost" sheetId="8" r:id="rId9"/>
     <sheet name="Region" sheetId="10" r:id="rId10"/>
-    <sheet name="TimeSlot" sheetId="13" r:id="rId11"/>
+    <sheet name="EDTSlot" sheetId="13" r:id="rId11"/>
+    <sheet name="UCTSlot" sheetId="14" r:id="rId12"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1048" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1069" uniqueCount="277">
   <si>
     <t>uid</t>
   </si>
@@ -798,68 +799,95 @@
   </si>
   <si>
     <t>for UC, ED</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>1, 1</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
-    <t>1, 1</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
     <t>1.005, 1.005</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>1.01, 1.01</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>1.015, 1.015</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>1.02, 1.02</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>1.025, 1.025</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>SLOT1</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>SLOT2</t>
-  </si>
-  <si>
-    <t>SLOT3</t>
-  </si>
-  <si>
-    <t>SLOT4</t>
-  </si>
-  <si>
-    <t>SLOT5</t>
-  </si>
-  <si>
-    <t>SLOT6</t>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>td1</t>
   </si>
   <si>
     <t>td2</t>
+  </si>
+  <si>
+    <t>1.005, 1.005</t>
+  </si>
+  <si>
+    <t>EDT1</t>
+  </si>
+  <si>
+    <t>EDT2</t>
+  </si>
+  <si>
+    <t>EDT3</t>
+  </si>
+  <si>
+    <t>EDT4</t>
+  </si>
+  <si>
+    <t>EDT5</t>
+  </si>
+  <si>
+    <t>EDT6</t>
+  </si>
+  <si>
+    <t>UCT1</t>
+  </si>
+  <si>
+    <t>UCT2</t>
+  </si>
+  <si>
+    <t>UCT3</t>
+  </si>
+  <si>
+    <t>UCT4</t>
+  </si>
+  <si>
+    <t>UCT5</t>
+  </si>
+  <si>
+    <t>UCT6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -907,7 +935,7 @@
     <font>
       <sz val="9"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -985,34 +1013,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1395,7 +1423,7 @@
       <c r="F2" s="5"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1453,7 +1481,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
@@ -1464,7 +1492,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1484,8 +1512,8 @@
       <c r="A2" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="10" t="s">
-        <v>262</v>
+      <c r="B2" s="13" t="s">
+        <v>265</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>256</v>
@@ -1495,8 +1523,8 @@
       <c r="A3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>263</v>
+      <c r="B3" s="13" t="s">
+        <v>266</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>257</v>
@@ -1506,8 +1534,8 @@
       <c r="A4" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="10" t="s">
-        <v>264</v>
+      <c r="B4" s="13" t="s">
+        <v>267</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>258</v>
@@ -1517,8 +1545,8 @@
       <c r="A5" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>265</v>
+      <c r="B5" s="13" t="s">
+        <v>268</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>259</v>
@@ -1528,8 +1556,8 @@
       <c r="A6" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="10" t="s">
-        <v>266</v>
+      <c r="B6" s="13" t="s">
+        <v>269</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>260</v>
@@ -1539,15 +1567,108 @@
       <c r="A7" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="10" t="s">
-        <v>267</v>
+      <c r="B7" s="13" t="s">
+        <v>270</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>261</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E8DE934-58E4-5047-A795-90496D563932}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>271</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>274</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>275</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>261</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2223,7 +2344,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <ignoredErrors>
@@ -2236,7 +2357,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:V5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="W23" sqref="W23"/>
     </sheetView>
   </sheetViews>
@@ -2306,11 +2427,11 @@
       <c r="T1" s="7" t="s">
         <v>254</v>
       </c>
-      <c r="U1" s="13" t="s">
-        <v>268</v>
-      </c>
-      <c r="V1" s="13" t="s">
-        <v>269</v>
+      <c r="U1" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="V1" s="12" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.2">
@@ -2574,7 +2695,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="A1:S5" numberStoredAsText="1"/>
@@ -2659,11 +2780,11 @@
       <c r="U1" s="7" t="s">
         <v>254</v>
       </c>
-      <c r="V1" s="11" t="s">
-        <v>268</v>
-      </c>
-      <c r="W1" s="11" t="s">
-        <v>269</v>
+      <c r="V1" s="10" t="s">
+        <v>262</v>
+      </c>
+      <c r="W1" s="10" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.2">
@@ -2727,15 +2848,15 @@
       <c r="U2" s="8">
         <v>1</v>
       </c>
-      <c r="V2" s="12">
+      <c r="V2" s="11">
         <v>50</v>
       </c>
-      <c r="W2" s="12">
+      <c r="W2" s="11">
         <v>30</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="A1:T2" numberStoredAsText="1"/>
@@ -3172,7 +3293,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="A1:K12" numberStoredAsText="1"/>
@@ -4628,7 +4749,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="A1:X21" numberStoredAsText="1"/>
@@ -4741,7 +4862,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="A1:J3" numberStoredAsText="1"/>
@@ -4802,7 +4923,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="A1:D3" numberStoredAsText="1"/>
@@ -4995,7 +5116,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="A1:D1 G1:I1 A6:D6 A2:D2 G2:I2 A3:D3 G3:I3 A4:D4 G4:I4 A5:D5 G5:I5 G6:I6" numberStoredAsText="1"/>

</xml_diff>

<commit_message>
Add data dt in timeslot
</commit_message>
<xml_diff>
--- a/ams/cases/ieee14/ieee14_uc.xlsx
+++ b/ams/cases/ieee14/ieee14_uc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinningwang/Documents/work/ams/ams/cases/ieee14/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60FD8622-7260-EE4F-A149-1E2B3811DC88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B96A8733-E9BE-0D46-A983-4225D15FC366}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36480" yWindow="1540" windowWidth="34560" windowHeight="19000" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-36480" yWindow="1540" windowWidth="34560" windowHeight="19000" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="12" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1069" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1071" uniqueCount="278">
   <si>
     <t>uid</t>
   </si>
@@ -869,6 +869,9 @@
   </si>
   <si>
     <t>UCT6</t>
+  </si>
+  <si>
+    <t>dt</t>
   </si>
 </sst>
 </file>
@@ -1489,15 +1492,15 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FD46B62-3884-454B-83D5-13A7DC1C4BB6}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1507,8 +1510,11 @@
       <c r="C1" s="6" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" s="13" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1518,8 +1524,11 @@
       <c r="C2" s="9" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1529,8 +1538,11 @@
       <c r="C3" s="9" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -1540,8 +1552,11 @@
       <c r="C4" s="9" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -1551,8 +1566,11 @@
       <c r="C5" s="9" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -1562,8 +1580,11 @@
       <c r="C6" s="9" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -1572,6 +1593,9 @@
       </c>
       <c r="C7" s="9" t="s">
         <v>261</v>
+      </c>
+      <c r="D7" s="1">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1582,15 +1606,15 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E8DE934-58E4-5047-A795-90496D563932}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R22" sqref="R22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1600,8 +1624,11 @@
       <c r="C1" s="6" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" s="13" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1611,8 +1638,11 @@
       <c r="C2" s="9" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1622,8 +1652,11 @@
       <c r="C3" s="9" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -1633,8 +1666,11 @@
       <c r="C4" s="9" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -1644,8 +1680,11 @@
       <c r="C5" s="9" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -1655,8 +1694,11 @@
       <c r="C6" s="9" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -1665,6 +1707,9 @@
       </c>
       <c r="C7" s="9" t="s">
         <v>261</v>
+      </c>
+      <c r="D7" s="1">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>